<commit_message>
Adds bearings from marks
</commit_message>
<xml_diff>
--- a/buoys_headings.xlsx
+++ b/buoys_headings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JackPreece\Code\Test scripts\for_fun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465EC6DE-58C9-4C98-93ED-28AD87291EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E4F67A-1747-4755-8475-325B34DE50C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,6 +523,9 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>238</v>
       </c>
@@ -576,6 +579,9 @@
       <c r="B3">
         <v>58</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="D3">
         <v>208</v>
       </c>
@@ -629,6 +635,9 @@
       <c r="C4">
         <v>28</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>35</v>
       </c>
@@ -682,6 +691,9 @@
       <c r="D5">
         <v>215</v>
       </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>227</v>
       </c>
@@ -735,6 +747,9 @@
       <c r="E6">
         <v>47</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
       <c r="G6">
         <v>37</v>
       </c>
@@ -788,6 +803,9 @@
       <c r="F7">
         <v>217</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7">
         <v>70</v>
       </c>
@@ -841,6 +859,9 @@
       <c r="G8">
         <v>250</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>308</v>
       </c>
@@ -894,6 +915,9 @@
       <c r="H9">
         <v>128</v>
       </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
       <c r="J9">
         <v>92</v>
       </c>
@@ -947,6 +971,9 @@
       <c r="I10">
         <v>272</v>
       </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
       <c r="K10">
         <v>233</v>
       </c>
@@ -1000,6 +1027,9 @@
       <c r="J11">
         <v>53</v>
       </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
       <c r="L11">
         <v>236</v>
       </c>
@@ -1053,6 +1083,9 @@
       <c r="K12">
         <v>56</v>
       </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
       <c r="M12">
         <v>46</v>
       </c>
@@ -1106,6 +1139,9 @@
       <c r="L13">
         <v>226</v>
       </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
       <c r="N13">
         <v>215</v>
       </c>
@@ -1159,6 +1195,9 @@
       <c r="M14">
         <v>35</v>
       </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
       <c r="O14">
         <v>275</v>
       </c>
@@ -1212,6 +1251,9 @@
       <c r="N15">
         <v>95</v>
       </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
       <c r="P15">
         <v>44</v>
       </c>
@@ -1265,11 +1307,14 @@
       <c r="O16">
         <v>224</v>
       </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
       <c r="Q16">
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1317,6 +1362,9 @@
       </c>
       <c r="P17">
         <v>48</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>